<commit_message>
getter 추가 및 app input부분 추가
</commit_message>
<xml_diff>
--- a/flight.xlsx
+++ b/flight.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\ascp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CEF12D1-DC7F-45F3-A87B-6D0470A2E89A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{036AF215-5280-40C0-BB64-236DCC763522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="615" windowWidth="15255" windowHeight="14865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10605" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="f" sheetId="1" r:id="rId1"/>
@@ -428,6 +428,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="177" formatCode="yyyy/mm/dd\ hh:mm:ss"/>
+  </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1018,7 +1021,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1379,12 +1382,13 @@
   <dimension ref="A1:G119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.25" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1395,13 +1399,13 @@
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F1" t="s">
@@ -3804,5 +3808,6 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>